<commit_message>
Updated datasets with duplicates removed.
</commit_message>
<xml_diff>
--- a/10250_0145.xlsx
+++ b/10250_0145.xlsx
@@ -9617,131 +9617,6 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId380"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>1</col>
-      <colOff>0</colOff>
-      <row>989</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="2438400" cy="2438400"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="381" name="Image 381" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId381"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>5</col>
-      <colOff>0</colOff>
-      <row>989</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="2438400" cy="2438400"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="382" name="Image 382" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId382"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>9</col>
-      <colOff>0</colOff>
-      <row>989</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="2438400" cy="2438400"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="383" name="Image 383" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId383"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>13</col>
-      <colOff>0</colOff>
-      <row>989</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="2438400" cy="2438400"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="384" name="Image 384" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId384"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>17</col>
-      <colOff>0</colOff>
-      <row>989</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="2438400" cy="2438400"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="385" name="Image 385" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId385"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -10044,7 +9919,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I78"/>
+  <dimension ref="A1:I77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12510,14 +12385,14 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>102.1996177_1.7223966_10250_0145_57</t>
+          <t>102.2226692_1.3842331_10250_0145_57</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>102.1996177</v>
+        <v>102.2226692</v>
       </c>
       <c r="C58" t="n">
-        <v>1.7223966</v>
+        <v>1.3842331</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -12526,41 +12401,41 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>cuts/102.1996177,1.7223966_10250_0145_RGB-composite.jpeg</t>
+          <t>cuts/102.2226692,1.3842331_10250_0145_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>cuts/102.1996177,1.7223966_10250_0145_Rojo-8micras.jpeg</t>
+          <t>cuts/102.2226692,1.3842331_10250_0145_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>cuts/102.1996177,1.7223966_10250_0145_I3-5.8micras.jpeg</t>
+          <t>cuts/102.2226692,1.3842331_10250_0145_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>cuts/102.1996177,1.7223966_10250_0145_Verde-4.6micras.jpeg</t>
+          <t>cuts/102.2226692,1.3842331_10250_0145_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>cuts/102.1996177,1.7223966_10250_0145_Azul-3.5micras.jpeg</t>
+          <t>cuts/102.2226692,1.3842331_10250_0145_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>102.2226692_1.3842331_10250_0145_58</t>
+          <t>102.2167069_1.0682322_10250_0145_58</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>102.2226692</v>
+        <v>102.2167069</v>
       </c>
       <c r="C59" t="n">
-        <v>1.3842331</v>
+        <v>1.0682322</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -12569,41 +12444,41 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>cuts/102.2226692,1.3842331_10250_0145_RGB-composite.jpeg</t>
+          <t>cuts/102.2167069,1.0682322_10250_0145_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>cuts/102.2226692,1.3842331_10250_0145_Rojo-8micras.jpeg</t>
+          <t>cuts/102.2167069,1.0682322_10250_0145_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>cuts/102.2226692,1.3842331_10250_0145_I3-5.8micras.jpeg</t>
+          <t>cuts/102.2167069,1.0682322_10250_0145_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>cuts/102.2226692,1.3842331_10250_0145_Verde-4.6micras.jpeg</t>
+          <t>cuts/102.2167069,1.0682322_10250_0145_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>cuts/102.2226692,1.3842331_10250_0145_Azul-3.5micras.jpeg</t>
+          <t>cuts/102.2167069,1.0682322_10250_0145_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>102.2167069_1.0682322_10250_0145_59</t>
+          <t>102.2991659_1.6730745_10250_0145_59</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>102.2167069</v>
+        <v>102.2991659</v>
       </c>
       <c r="C60" t="n">
-        <v>1.0682322</v>
+        <v>1.6730745</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -12612,41 +12487,41 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>cuts/102.2167069,1.0682322_10250_0145_RGB-composite.jpeg</t>
+          <t>cuts/102.2991659,1.6730745_10250_0145_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>cuts/102.2167069,1.0682322_10250_0145_Rojo-8micras.jpeg</t>
+          <t>cuts/102.2991659,1.6730745_10250_0145_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>cuts/102.2167069,1.0682322_10250_0145_I3-5.8micras.jpeg</t>
+          <t>cuts/102.2991659,1.6730745_10250_0145_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>cuts/102.2167069,1.0682322_10250_0145_Verde-4.6micras.jpeg</t>
+          <t>cuts/102.2991659,1.6730745_10250_0145_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>cuts/102.2167069,1.0682322_10250_0145_Azul-3.5micras.jpeg</t>
+          <t>cuts/102.2991659,1.6730745_10250_0145_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>102.2991659_1.6730745_10250_0145_60</t>
+          <t>102.2916625_1.6765739_10250_0145_60</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>102.2991659</v>
+        <v>102.2916625</v>
       </c>
       <c r="C61" t="n">
-        <v>1.6730745</v>
+        <v>1.6765739</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
@@ -12655,41 +12530,41 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>cuts/102.2991659,1.6730745_10250_0145_RGB-composite.jpeg</t>
+          <t>cuts/102.2916625,1.6765739_10250_0145_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>cuts/102.2991659,1.6730745_10250_0145_Rojo-8micras.jpeg</t>
+          <t>cuts/102.2916625,1.6765739_10250_0145_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>cuts/102.2991659,1.6730745_10250_0145_I3-5.8micras.jpeg</t>
+          <t>cuts/102.2916625,1.6765739_10250_0145_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>cuts/102.2991659,1.6730745_10250_0145_Verde-4.6micras.jpeg</t>
+          <t>cuts/102.2916625,1.6765739_10250_0145_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>cuts/102.2991659,1.6730745_10250_0145_Azul-3.5micras.jpeg</t>
+          <t>cuts/102.2916625,1.6765739_10250_0145_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>102.2916625_1.6765739_10250_0145_61</t>
+          <t>102.4505567_1.9490827_10250_0145_61</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>102.2916625</v>
+        <v>102.4505567</v>
       </c>
       <c r="C62" t="n">
-        <v>1.6765739</v>
+        <v>1.9490827</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -12698,41 +12573,41 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>cuts/102.2916625,1.6765739_10250_0145_RGB-composite.jpeg</t>
+          <t>cuts/102.4505567,1.9490827_10250_0145_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>cuts/102.2916625,1.6765739_10250_0145_Rojo-8micras.jpeg</t>
+          <t>cuts/102.4505567,1.9490827_10250_0145_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>cuts/102.2916625,1.6765739_10250_0145_I3-5.8micras.jpeg</t>
+          <t>cuts/102.4505567,1.9490827_10250_0145_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>cuts/102.2916625,1.6765739_10250_0145_Verde-4.6micras.jpeg</t>
+          <t>cuts/102.4505567,1.9490827_10250_0145_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>cuts/102.2916625,1.6765739_10250_0145_Azul-3.5micras.jpeg</t>
+          <t>cuts/102.4505567,1.9490827_10250_0145_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>102.4505567_1.9490827_10250_0145_62</t>
+          <t>102.4313850_1.7725822_10250_0145_62</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>102.4505567</v>
+        <v>102.431385</v>
       </c>
       <c r="C63" t="n">
-        <v>1.9490827</v>
+        <v>1.7725822</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
@@ -12741,41 +12616,41 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>cuts/102.4505567,1.9490827_10250_0145_RGB-composite.jpeg</t>
+          <t>cuts/102.4313850,1.7725822_10250_0145_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>cuts/102.4505567,1.9490827_10250_0145_Rojo-8micras.jpeg</t>
+          <t>cuts/102.4313850,1.7725822_10250_0145_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>cuts/102.4505567,1.9490827_10250_0145_I3-5.8micras.jpeg</t>
+          <t>cuts/102.4313850,1.7725822_10250_0145_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>cuts/102.4505567,1.9490827_10250_0145_Verde-4.6micras.jpeg</t>
+          <t>cuts/102.4313850,1.7725822_10250_0145_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>cuts/102.4505567,1.9490827_10250_0145_Azul-3.5micras.jpeg</t>
+          <t>cuts/102.4313850,1.7725822_10250_0145_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>102.4313850_1.7725822_10250_0145_63</t>
+          <t>102.3185694_0.8984094_10250_0145_63</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>102.431385</v>
+        <v>102.3185694</v>
       </c>
       <c r="C64" t="n">
-        <v>1.7725822</v>
+        <v>0.8984094</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
@@ -12784,41 +12659,41 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>cuts/102.4313850,1.7725822_10250_0145_RGB-composite.jpeg</t>
+          <t>cuts/102.3185694,0.8984094_10250_0145_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>cuts/102.4313850,1.7725822_10250_0145_Rojo-8micras.jpeg</t>
+          <t>cuts/102.3185694,0.8984094_10250_0145_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>cuts/102.4313850,1.7725822_10250_0145_I3-5.8micras.jpeg</t>
+          <t>cuts/102.3185694,0.8984094_10250_0145_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>cuts/102.4313850,1.7725822_10250_0145_Verde-4.6micras.jpeg</t>
+          <t>cuts/102.3185694,0.8984094_10250_0145_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>cuts/102.4313850,1.7725822_10250_0145_Azul-3.5micras.jpeg</t>
+          <t>cuts/102.3185694,0.8984094_10250_0145_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>102.3185694_0.8984094_10250_0145_64</t>
+          <t>102.4737489_0.8304167_10250_0145_64</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>102.3185694</v>
+        <v>102.4737489</v>
       </c>
       <c r="C65" t="n">
-        <v>0.8984094</v>
+        <v>0.8304167</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
@@ -12827,41 +12702,41 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>cuts/102.3185694,0.8984094_10250_0145_RGB-composite.jpeg</t>
+          <t>cuts/102.4737489,0.8304167_10250_0145_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>cuts/102.3185694,0.8984094_10250_0145_Rojo-8micras.jpeg</t>
+          <t>cuts/102.4737489,0.8304167_10250_0145_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>cuts/102.3185694,0.8984094_10250_0145_I3-5.8micras.jpeg</t>
+          <t>cuts/102.4737489,0.8304167_10250_0145_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>cuts/102.3185694,0.8984094_10250_0145_Verde-4.6micras.jpeg</t>
+          <t>cuts/102.4737489,0.8304167_10250_0145_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>cuts/102.3185694,0.8984094_10250_0145_Azul-3.5micras.jpeg</t>
+          <t>cuts/102.4737489,0.8304167_10250_0145_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>102.4737489_0.8304167_10250_0145_65</t>
+          <t>102.4897590_1.2131944_10250_0145_65</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>102.4737489</v>
+        <v>102.489759</v>
       </c>
       <c r="C66" t="n">
-        <v>0.8304167</v>
+        <v>1.2131944</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
@@ -12870,41 +12745,41 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>cuts/102.4737489,0.8304167_10250_0145_RGB-composite.jpeg</t>
+          <t>cuts/102.4897590,1.2131944_10250_0145_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>cuts/102.4737489,0.8304167_10250_0145_Rojo-8micras.jpeg</t>
+          <t>cuts/102.4897590,1.2131944_10250_0145_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>cuts/102.4737489,0.8304167_10250_0145_I3-5.8micras.jpeg</t>
+          <t>cuts/102.4897590,1.2131944_10250_0145_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>cuts/102.4737489,0.8304167_10250_0145_Verde-4.6micras.jpeg</t>
+          <t>cuts/102.4897590,1.2131944_10250_0145_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>cuts/102.4737489,0.8304167_10250_0145_Azul-3.5micras.jpeg</t>
+          <t>cuts/102.4897590,1.2131944_10250_0145_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>102.4897590_1.2131944_10250_0145_66</t>
+          <t>102.5734550_1.8575036_10250_0145_66</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>102.489759</v>
+        <v>102.573455</v>
       </c>
       <c r="C67" t="n">
-        <v>1.2131944</v>
+        <v>1.8575036</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
@@ -12913,41 +12788,41 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>cuts/102.4897590,1.2131944_10250_0145_RGB-composite.jpeg</t>
+          <t>cuts/102.5734550,1.8575036_10250_0145_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>cuts/102.4897590,1.2131944_10250_0145_Rojo-8micras.jpeg</t>
+          <t>cuts/102.5734550,1.8575036_10250_0145_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>cuts/102.4897590,1.2131944_10250_0145_I3-5.8micras.jpeg</t>
+          <t>cuts/102.5734550,1.8575036_10250_0145_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>cuts/102.4897590,1.2131944_10250_0145_Verde-4.6micras.jpeg</t>
+          <t>cuts/102.5734550,1.8575036_10250_0145_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t>cuts/102.4897590,1.2131944_10250_0145_Azul-3.5micras.jpeg</t>
+          <t>cuts/102.5734550,1.8575036_10250_0145_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>102.5734550_1.8575036_10250_0145_67</t>
+          <t>102.7498467_1.8517920_10250_0145_67</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>102.573455</v>
+        <v>102.7498467</v>
       </c>
       <c r="C68" t="n">
-        <v>1.8575036</v>
+        <v>1.851792</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
@@ -12956,41 +12831,41 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>cuts/102.5734550,1.8575036_10250_0145_RGB-composite.jpeg</t>
+          <t>cuts/102.7498467,1.8517920_10250_0145_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>cuts/102.5734550,1.8575036_10250_0145_Rojo-8micras.jpeg</t>
+          <t>cuts/102.7498467,1.8517920_10250_0145_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>cuts/102.5734550,1.8575036_10250_0145_I3-5.8micras.jpeg</t>
+          <t>cuts/102.7498467,1.8517920_10250_0145_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>cuts/102.5734550,1.8575036_10250_0145_Verde-4.6micras.jpeg</t>
+          <t>cuts/102.7498467,1.8517920_10250_0145_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>cuts/102.5734550,1.8575036_10250_0145_Azul-3.5micras.jpeg</t>
+          <t>cuts/102.7498467,1.8517920_10250_0145_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>102.7498467_1.8517920_10250_0145_68</t>
+          <t>102.7394946_1.7230984_10250_0145_68</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>102.7498467</v>
+        <v>102.7394946</v>
       </c>
       <c r="C69" t="n">
-        <v>1.851792</v>
+        <v>1.7230984</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
@@ -12999,41 +12874,41 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>cuts/102.7498467,1.8517920_10250_0145_RGB-composite.jpeg</t>
+          <t>cuts/102.7394946,1.7230984_10250_0145_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>cuts/102.7498467,1.8517920_10250_0145_Rojo-8micras.jpeg</t>
+          <t>cuts/102.7394946,1.7230984_10250_0145_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>cuts/102.7498467,1.8517920_10250_0145_I3-5.8micras.jpeg</t>
+          <t>cuts/102.7394946,1.7230984_10250_0145_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>cuts/102.7498467,1.8517920_10250_0145_Verde-4.6micras.jpeg</t>
+          <t>cuts/102.7394946,1.7230984_10250_0145_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>cuts/102.7498467,1.8517920_10250_0145_Azul-3.5micras.jpeg</t>
+          <t>cuts/102.7394946,1.7230984_10250_0145_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>102.7394946_1.7230984_10250_0145_69</t>
+          <t>102.8307933_1.0211148_10250_0145_69</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>102.7394946</v>
+        <v>102.8307933</v>
       </c>
       <c r="C70" t="n">
-        <v>1.7230984</v>
+        <v>1.0211148</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
@@ -13042,41 +12917,41 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>cuts/102.7394946,1.7230984_10250_0145_RGB-composite.jpeg</t>
+          <t>cuts/102.8307933,1.0211148_10250_0145_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>cuts/102.7394946,1.7230984_10250_0145_Rojo-8micras.jpeg</t>
+          <t>cuts/102.8307933,1.0211148_10250_0145_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>cuts/102.7394946,1.7230984_10250_0145_I3-5.8micras.jpeg</t>
+          <t>cuts/102.8307933,1.0211148_10250_0145_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>cuts/102.7394946,1.7230984_10250_0145_Verde-4.6micras.jpeg</t>
+          <t>cuts/102.8307933,1.0211148_10250_0145_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I70" t="inlineStr">
         <is>
-          <t>cuts/102.7394946,1.7230984_10250_0145_Azul-3.5micras.jpeg</t>
+          <t>cuts/102.8307933,1.0211148_10250_0145_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>102.8307933_1.0211148_10250_0145_70</t>
+          <t>102.2164111_1.5672323_10250_0145_70</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>102.8307933</v>
+        <v>102.2164111</v>
       </c>
       <c r="C71" t="n">
-        <v>1.0211148</v>
+        <v>1.5672323</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
@@ -13085,41 +12960,41 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>cuts/102.8307933,1.0211148_10250_0145_RGB-composite.jpeg</t>
+          <t>cuts/102.2164111,1.5672323_10250_0145_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>cuts/102.8307933,1.0211148_10250_0145_Rojo-8micras.jpeg</t>
+          <t>cuts/102.2164111,1.5672323_10250_0145_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>cuts/102.8307933,1.0211148_10250_0145_I3-5.8micras.jpeg</t>
+          <t>cuts/102.2164111,1.5672323_10250_0145_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>cuts/102.8307933,1.0211148_10250_0145_Verde-4.6micras.jpeg</t>
+          <t>cuts/102.2164111,1.5672323_10250_0145_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I71" t="inlineStr">
         <is>
-          <t>cuts/102.8307933,1.0211148_10250_0145_Azul-3.5micras.jpeg</t>
+          <t>cuts/102.2164111,1.5672323_10250_0145_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>102.2164111_1.5672323_10250_0145_71</t>
+          <t>102.0585893_1.2755737_10250_0145_71</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>102.2164111</v>
+        <v>102.0585893</v>
       </c>
       <c r="C72" t="n">
-        <v>1.5672323</v>
+        <v>1.2755737</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
@@ -13128,41 +13003,41 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>cuts/102.2164111,1.5672323_10250_0145_RGB-composite.jpeg</t>
+          <t>cuts/102.0585893,1.2755737_10250_0145_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>cuts/102.2164111,1.5672323_10250_0145_Rojo-8micras.jpeg</t>
+          <t>cuts/102.0585893,1.2755737_10250_0145_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>cuts/102.2164111,1.5672323_10250_0145_I3-5.8micras.jpeg</t>
+          <t>cuts/102.0585893,1.2755737_10250_0145_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>cuts/102.2164111,1.5672323_10250_0145_Verde-4.6micras.jpeg</t>
+          <t>cuts/102.0585893,1.2755737_10250_0145_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I72" t="inlineStr">
         <is>
-          <t>cuts/102.2164111,1.5672323_10250_0145_Azul-3.5micras.jpeg</t>
+          <t>cuts/102.0585893,1.2755737_10250_0145_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>102.0585893_1.2755737_10250_0145_72</t>
+          <t>102.0378606_2.0964427_10250_0145_72</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>102.0585893</v>
+        <v>102.0378606</v>
       </c>
       <c r="C73" t="n">
-        <v>1.2755737</v>
+        <v>2.0964427</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
@@ -13171,41 +13046,41 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>cuts/102.0585893,1.2755737_10250_0145_RGB-composite.jpeg</t>
+          <t>cuts/102.0378606,2.0964427_10250_0145_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>cuts/102.0585893,1.2755737_10250_0145_Rojo-8micras.jpeg</t>
+          <t>cuts/102.0378606,2.0964427_10250_0145_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>cuts/102.0585893,1.2755737_10250_0145_I3-5.8micras.jpeg</t>
+          <t>cuts/102.0378606,2.0964427_10250_0145_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>cuts/102.0585893,1.2755737_10250_0145_Verde-4.6micras.jpeg</t>
+          <t>cuts/102.0378606,2.0964427_10250_0145_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I73" t="inlineStr">
         <is>
-          <t>cuts/102.0585893,1.2755737_10250_0145_Azul-3.5micras.jpeg</t>
+          <t>cuts/102.0378606,2.0964427_10250_0145_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>102.0378606_2.0964427_10250_0145_73</t>
+          <t>102.7350668_0.8872380_10250_0145_73</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>102.0378606</v>
+        <v>102.7350668</v>
       </c>
       <c r="C74" t="n">
-        <v>2.0964427</v>
+        <v>0.887238</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
@@ -13214,41 +13089,41 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>cuts/102.0378606,2.0964427_10250_0145_RGB-composite.jpeg</t>
+          <t>cuts/102.7350668,0.8872380_10250_0145_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>cuts/102.0378606,2.0964427_10250_0145_Rojo-8micras.jpeg</t>
+          <t>cuts/102.7350668,0.8872380_10250_0145_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>cuts/102.0378606,2.0964427_10250_0145_I3-5.8micras.jpeg</t>
+          <t>cuts/102.7350668,0.8872380_10250_0145_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>cuts/102.0378606,2.0964427_10250_0145_Verde-4.6micras.jpeg</t>
+          <t>cuts/102.7350668,0.8872380_10250_0145_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I74" t="inlineStr">
         <is>
-          <t>cuts/102.0378606,2.0964427_10250_0145_Azul-3.5micras.jpeg</t>
+          <t>cuts/102.7350668,0.8872380_10250_0145_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>102.7350668_0.8872380_10250_0145_74</t>
+          <t>102.5938288_0.8412628_10250_0145_74</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>102.7350668</v>
+        <v>102.5938288</v>
       </c>
       <c r="C75" t="n">
-        <v>0.887238</v>
+        <v>0.8412628</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
@@ -13257,41 +13132,41 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>cuts/102.7350668,0.8872380_10250_0145_RGB-composite.jpeg</t>
+          <t>cuts/102.5938288,0.8412628_10250_0145_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>cuts/102.7350668,0.8872380_10250_0145_Rojo-8micras.jpeg</t>
+          <t>cuts/102.5938288,0.8412628_10250_0145_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>cuts/102.7350668,0.8872380_10250_0145_I3-5.8micras.jpeg</t>
+          <t>cuts/102.5938288,0.8412628_10250_0145_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>cuts/102.7350668,0.8872380_10250_0145_Verde-4.6micras.jpeg</t>
+          <t>cuts/102.5938288,0.8412628_10250_0145_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I75" t="inlineStr">
         <is>
-          <t>cuts/102.7350668,0.8872380_10250_0145_Azul-3.5micras.jpeg</t>
+          <t>cuts/102.5938288,0.8412628_10250_0145_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>102.5938288_0.8412628_10250_0145_75</t>
+          <t>101.9533198_1.6487538_10250_0145_75</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>102.5938288</v>
+        <v>101.9533198</v>
       </c>
       <c r="C76" t="n">
-        <v>0.8412628</v>
+        <v>1.6487538</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
@@ -13300,41 +13175,41 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>cuts/102.5938288,0.8412628_10250_0145_RGB-composite.jpeg</t>
+          <t>cuts/101.9533198,1.6487538_10250_0145_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>cuts/102.5938288,0.8412628_10250_0145_Rojo-8micras.jpeg</t>
+          <t>cuts/101.9533198,1.6487538_10250_0145_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>cuts/102.5938288,0.8412628_10250_0145_I3-5.8micras.jpeg</t>
+          <t>cuts/101.9533198,1.6487538_10250_0145_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>cuts/102.5938288,0.8412628_10250_0145_Verde-4.6micras.jpeg</t>
+          <t>cuts/101.9533198,1.6487538_10250_0145_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I76" t="inlineStr">
         <is>
-          <t>cuts/102.5938288,0.8412628_10250_0145_Azul-3.5micras.jpeg</t>
+          <t>cuts/101.9533198,1.6487538_10250_0145_Azul-3.5micras.jpeg</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>101.9533198_1.6487538_10250_0145_76</t>
+          <t>101.9800950_1.6433850_10250_0145_76</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>101.9533198</v>
+        <v>101.980095</v>
       </c>
       <c r="C77" t="n">
-        <v>1.6487538</v>
+        <v>1.643385</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
@@ -13343,68 +13218,25 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>cuts/101.9533198,1.6487538_10250_0145_RGB-composite.jpeg</t>
+          <t>cuts/101.9800950,1.6433850_10250_0145_RGB-composite.jpeg</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>cuts/101.9533198,1.6487538_10250_0145_Rojo-8micras.jpeg</t>
+          <t>cuts/101.9800950,1.6433850_10250_0145_Rojo-8micras.jpeg</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>cuts/101.9533198,1.6487538_10250_0145_I3-5.8micras.jpeg</t>
+          <t>cuts/101.9800950,1.6433850_10250_0145_I3-5.8micras.jpeg</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>cuts/101.9533198,1.6487538_10250_0145_Verde-4.6micras.jpeg</t>
+          <t>cuts/101.9800950,1.6433850_10250_0145_Verde-4.6micras.jpeg</t>
         </is>
       </c>
       <c r="I77" t="inlineStr">
-        <is>
-          <t>cuts/101.9533198,1.6487538_10250_0145_Azul-3.5micras.jpeg</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>101.9800950_1.6433850_10250_0145_77</t>
-        </is>
-      </c>
-      <c r="B78" t="n">
-        <v>101.980095</v>
-      </c>
-      <c r="C78" t="n">
-        <v>1.643385</v>
-      </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>cuts/101.9800950,1.6433850_10250_0145_RGB-composite.jpeg</t>
-        </is>
-      </c>
-      <c r="F78" t="inlineStr">
-        <is>
-          <t>cuts/101.9800950,1.6433850_10250_0145_Rojo-8micras.jpeg</t>
-        </is>
-      </c>
-      <c r="G78" t="inlineStr">
-        <is>
-          <t>cuts/101.9800950,1.6433850_10250_0145_I3-5.8micras.jpeg</t>
-        </is>
-      </c>
-      <c r="H78" t="inlineStr">
-        <is>
-          <t>cuts/101.9800950,1.6433850_10250_0145_Verde-4.6micras.jpeg</t>
-        </is>
-      </c>
-      <c r="I78" t="inlineStr">
         <is>
           <t>cuts/101.9800950,1.6433850_10250_0145_Azul-3.5micras.jpeg</t>
         </is>
@@ -13421,7 +13253,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R990"/>
+  <dimension ref="A1:R977"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13868,147 +13700,140 @@
     <row r="730">
       <c r="A730" t="inlineStr">
         <is>
-          <t>102.1996177_1.7223966_10250_0145_57</t>
+          <t>102.2226692_1.3842331_10250_0145_57</t>
         </is>
       </c>
     </row>
     <row r="743">
       <c r="A743" t="inlineStr">
         <is>
-          <t>102.2226692_1.3842331_10250_0145_58</t>
+          <t>102.2167069_1.0682322_10250_0145_58</t>
         </is>
       </c>
     </row>
     <row r="756">
       <c r="A756" t="inlineStr">
         <is>
-          <t>102.2167069_1.0682322_10250_0145_59</t>
+          <t>102.2991659_1.6730745_10250_0145_59</t>
         </is>
       </c>
     </row>
     <row r="769">
       <c r="A769" t="inlineStr">
         <is>
-          <t>102.2991659_1.6730745_10250_0145_60</t>
+          <t>102.2916625_1.6765739_10250_0145_60</t>
         </is>
       </c>
     </row>
     <row r="782">
       <c r="A782" t="inlineStr">
         <is>
-          <t>102.2916625_1.6765739_10250_0145_61</t>
+          <t>102.4505567_1.9490827_10250_0145_61</t>
         </is>
       </c>
     </row>
     <row r="795">
       <c r="A795" t="inlineStr">
         <is>
-          <t>102.4505567_1.9490827_10250_0145_62</t>
+          <t>102.4313850_1.7725822_10250_0145_62</t>
         </is>
       </c>
     </row>
     <row r="808">
       <c r="A808" t="inlineStr">
         <is>
-          <t>102.4313850_1.7725822_10250_0145_63</t>
+          <t>102.3185694_0.8984094_10250_0145_63</t>
         </is>
       </c>
     </row>
     <row r="821">
       <c r="A821" t="inlineStr">
         <is>
-          <t>102.3185694_0.8984094_10250_0145_64</t>
+          <t>102.4737489_0.8304167_10250_0145_64</t>
         </is>
       </c>
     </row>
     <row r="834">
       <c r="A834" t="inlineStr">
         <is>
-          <t>102.4737489_0.8304167_10250_0145_65</t>
+          <t>102.4897590_1.2131944_10250_0145_65</t>
         </is>
       </c>
     </row>
     <row r="847">
       <c r="A847" t="inlineStr">
         <is>
-          <t>102.4897590_1.2131944_10250_0145_66</t>
+          <t>102.5734550_1.8575036_10250_0145_66</t>
         </is>
       </c>
     </row>
     <row r="860">
       <c r="A860" t="inlineStr">
         <is>
-          <t>102.5734550_1.8575036_10250_0145_67</t>
+          <t>102.7498467_1.8517920_10250_0145_67</t>
         </is>
       </c>
     </row>
     <row r="873">
       <c r="A873" t="inlineStr">
         <is>
-          <t>102.7498467_1.8517920_10250_0145_68</t>
+          <t>102.7394946_1.7230984_10250_0145_68</t>
         </is>
       </c>
     </row>
     <row r="886">
       <c r="A886" t="inlineStr">
         <is>
-          <t>102.7394946_1.7230984_10250_0145_69</t>
+          <t>102.8307933_1.0211148_10250_0145_69</t>
         </is>
       </c>
     </row>
     <row r="899">
       <c r="A899" t="inlineStr">
         <is>
-          <t>102.8307933_1.0211148_10250_0145_70</t>
+          <t>102.2164111_1.5672323_10250_0145_70</t>
         </is>
       </c>
     </row>
     <row r="912">
       <c r="A912" t="inlineStr">
         <is>
-          <t>102.2164111_1.5672323_10250_0145_71</t>
+          <t>102.0585893_1.2755737_10250_0145_71</t>
         </is>
       </c>
     </row>
     <row r="925">
       <c r="A925" t="inlineStr">
         <is>
-          <t>102.0585893_1.2755737_10250_0145_72</t>
+          <t>102.0378606_2.0964427_10250_0145_72</t>
         </is>
       </c>
     </row>
     <row r="938">
       <c r="A938" t="inlineStr">
         <is>
-          <t>102.0378606_2.0964427_10250_0145_73</t>
+          <t>102.7350668_0.8872380_10250_0145_73</t>
         </is>
       </c>
     </row>
     <row r="951">
       <c r="A951" t="inlineStr">
         <is>
-          <t>102.7350668_0.8872380_10250_0145_74</t>
+          <t>102.5938288_0.8412628_10250_0145_74</t>
         </is>
       </c>
     </row>
     <row r="964">
       <c r="A964" t="inlineStr">
         <is>
-          <t>102.5938288_0.8412628_10250_0145_75</t>
+          <t>101.9533198_1.6487538_10250_0145_75</t>
         </is>
       </c>
     </row>
     <row r="977">
       <c r="A977" t="inlineStr">
         <is>
-          <t>101.9533198_1.6487538_10250_0145_76</t>
-        </is>
-      </c>
-    </row>
-    <row r="990">
-      <c r="A990" t="inlineStr">
-        <is>
-          <t>101.9800950_1.6433850_10250_0145_77</t>
+          <t>101.9800950_1.6433850_10250_0145_76</t>
         </is>
       </c>
     </row>

</xml_diff>